<commit_message>
Data Driven concept applied to some methods
</commit_message>
<xml_diff>
--- a/makeMyTripAutomation/HackathonData.xlsx
+++ b/makeMyTripAutomation/HackathonData.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A7D5FA57-86C8-4CEE-B9C5-95ACFF44F0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3bf01c7e740b79e1/Documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{74A6EF7D-B499-4DAD-B396-E28CA8F1447E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1B0A574-21A8-47AE-BE35-467D4E733E71}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{58ACEAC8-737A-4424-A999-F5AF1A6DC674}"/>
   </bookViews>
@@ -11,8 +16,7 @@
     <sheet name="readData" sheetId="1" r:id="rId1"/>
     <sheet name="writeData" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>URL</t>
   </si>
@@ -46,14 +50,58 @@
   </si>
   <si>
     <t>Adults Size</t>
+  </si>
+  <si>
+    <t>Extent report name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make My Trip Hackathon </t>
+  </si>
+  <si>
+    <t>Login Id</t>
+  </si>
+  <si>
+    <t>bughunterss01@gmail.com</t>
+  </si>
+  <si>
+    <t>Login Password</t>
+  </si>
+  <si>
+    <t>Bughunter$6</t>
+  </si>
+  <si>
+    <t>PopUp Title</t>
+  </si>
+  <si>
+    <t>Login/Signup for Best Prices</t>
+  </si>
+  <si>
+    <t>Departure city input</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Arrival City Input</t>
+  </si>
+  <si>
+    <t>Manali</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -81,9 +129,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -400,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89CCFE8B-D895-46EC-A635-DF862E4E2EEF}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,18 +462,36 @@
     <col min="1" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -431,10 +500,29 @@
       </c>
       <c r="C2" s="1">
         <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Final commit for 11 july
</commit_message>
<xml_diff>
--- a/makeMyTripAutomation/HackathonData.xlsx
+++ b/makeMyTripAutomation/HackathonData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3bf01c7e740b79e1/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{74A6EF7D-B499-4DAD-B396-E28CA8F1447E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1B0A574-21A8-47AE-BE35-467D4E733E71}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{74A6EF7D-B499-4DAD-B396-E28CA8F1447E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A064470-6BC9-4461-92A4-54B187B3F6E7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{58ACEAC8-737A-4424-A999-F5AF1A6DC674}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>URL</t>
   </si>
@@ -86,6 +86,15 @@
   </si>
   <si>
     <t>Manali</t>
+  </si>
+  <si>
+    <t>Departure date input</t>
+  </si>
+  <si>
+    <t>Login Name</t>
+  </si>
+  <si>
+    <t>Hey Bug Hunters</t>
   </si>
 </sst>
 </file>
@@ -451,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89CCFE8B-D895-46EC-A635-DF862E4E2EEF}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,7 +471,7 @@
     <col min="1" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -490,8 +499,14 @@
       <c r="I1" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -518,6 +533,12 @@
       </c>
       <c r="I2" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="J2" s="1">
+        <v>20</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit 3 12 july
</commit_message>
<xml_diff>
--- a/makeMyTripAutomation/HackathonData.xlsx
+++ b/makeMyTripAutomation/HackathonData.xlsx
@@ -3,12 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3bf01c7e740b79e1/Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{74A6EF7D-B499-4DAD-B396-E28CA8F1447E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A064470-6BC9-4461-92A4-54B187B3F6E7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{540FECFF-5D2B-46F5-9B47-9FC40E6EEB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{58ACEAC8-737A-4424-A999-F5AF1A6DC674}"/>
   </bookViews>
@@ -16,7 +11,8 @@
     <sheet name="readData" sheetId="1" r:id="rId1"/>
     <sheet name="writeData" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>URL</t>
   </si>
@@ -95,13 +91,28 @@
   </si>
   <si>
     <t>Hey Bug Hunters</t>
+  </si>
+  <si>
+    <t>Gift card Input 1</t>
+  </si>
+  <si>
+    <t>Gift card Input 2</t>
+  </si>
+  <si>
+    <t>Gift card Input 3</t>
+  </si>
+  <si>
+    <t>BugHunters</t>
+  </si>
+  <si>
+    <t>test@gmail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +124,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,10 +160,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -146,8 +172,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -460,15 +490,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89CCFE8B-D895-46EC-A635-DF862E4E2EEF}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -541,9 +573,35 @@
         <v>19</v>
       </c>
     </row>
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9999999562</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{0E3F8651-3A02-4AF6-99C5-C8242049C16B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>